<commit_message>
styles & formulas copying
</commit_message>
<xml_diff>
--- a/WriteTestBook.xlsx
+++ b/WriteTestBook.xlsx
@@ -1,29 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ivan\ObjectStyle\tmpProjects\ApachePOITest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivannikitka/IdeaProjects/ ObjectStyle/tmp/ApachePOITest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE12920-C106-4EFB-BF4F-920E1F7699A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5F1388-0FEB-0545-BF6E-B8887263E830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14240" xr2:uid="{D9696ABA-CDAC-264D-8BCE-8FDC23B0FCD9}"/>
   </bookViews>
   <sheets>
-    <sheet name="19th century artists" sheetId="1" r:id="rId1"/>
-    <sheet name="20th century artists" sheetId="2" r:id="rId2"/>
+    <sheet name="Artist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>id</t>
   </si>
@@ -39,47 +44,45 @@
     <t>ARTIST_NAME</t>
   </si>
   <si>
-    <t>DATE_OF_BIRTH</t>
+    <t>YEAR_OF_BIRTH</t>
+  </si>
+  <si>
+    <t>AGE</t>
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Salvador Dali</t>
-  </si>
-  <si>
-    <t>11 May 1904</t>
-  </si>
-  <si>
-    <t>Andy Warhol</t>
-  </si>
-  <si>
-    <t>6 August 1928</t>
-  </si>
-  <si>
-    <t>Pablo Picasso</t>
-  </si>
-  <si>
-    <t>25 October 1881</t>
-  </si>
-  <si>
-    <t>Marc Chagall</t>
-  </si>
-  <si>
-    <t>24 June 1887</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -87,50 +90,92 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -139,79 +184,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
-        <charset val="204"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <charset val="204"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <charset val="204"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -224,24 +245,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D5AADEE2-4404-4E54-ABDF-4EE5AE7DF24E}" name="Artist19" displayName="Artist19" ref="G16:I17" totalsRowShown="0">
-  <autoFilter ref="G16:I17" xr:uid="{D5AADEE2-4404-4E54-ABDF-4EE5AE7DF24E}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{735E9C80-BCE4-478A-88F4-BE203126EB66}" name="id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{25CF12A5-AD27-4A1A-98D4-744C657941F9}" name="ARTIST_NAME" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{985DCFCC-5C9B-417F-939D-728FCDE1A0E4}" name="DATE_OF_BIRTH" dataDxfId="3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE22F780-88F0-42D4-885E-432F8AA09996}" name="Artist20" displayName="Artist20" ref="C14:E15" totalsRowShown="0">
-  <autoFilter ref="C14:E15" xr:uid="{CE22F780-88F0-42D4-885E-432F8AA09996}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EAC012F2-FEC7-4E8A-9719-904DD09940F2}" name="id" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{6C2061DB-1CB4-4F64-9486-E59FCCBCB969}" name="ARTIST_NAME" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{96C25854-589A-452E-8C96-21932DADF90B}" name="DATE_OF_BIRTH" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B526177E-D28F-8B40-855A-0AF30101F4C4}" name="Artist" displayName="Artist" ref="C6:F8" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="C6:F8" xr:uid="{B526177E-D28F-8B40-855A-0AF30101F4C4}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{24C2B1A5-AA3F-5B47-A3BE-F7B8C219B519}" name="id"/>
+    <tableColumn id="2" xr3:uid="{1C566B9C-3DC9-C144-8C8E-DF47015BD160}" name="ARTIST_NAME"/>
+    <tableColumn id="3" xr3:uid="{964F1121-50D9-7A44-BE4F-9AC38F2CC6AD}" name="YEAR_OF_BIRTH"/>
+    <tableColumn id="4" xr3:uid="{66ADC7EE-4108-914D-ABF0-23C2C2F021A4}" name="AGE">
+      <calculatedColumnFormula>2023-Artist!$E7</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -543,164 +555,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G16:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36E4FD2-C194-4040-A648-48D601BE96A2}">
+  <dimension ref="C6:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.140625"/>
-    <col min="2" max="2" customWidth="true" width="17.85546875"/>
-    <col min="3" max="3" customWidth="true" width="21.7109375"/>
-    <col min="7" max="7" customWidth="true" width="13.0"/>
-    <col min="8" max="8" customWidth="true" width="17.28515625"/>
-    <col min="9" max="9" customWidth="true" width="32.7109375"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G16" s="1" t="s">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H16" t="s" s="0">
+      <c r="D6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I16" t="s" s="0">
+      <c r="E6" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G17" s="3">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="G18" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="H18" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="I18" t="s" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="G19" t="n" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="H19" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="I19" t="s" s="0">
-        <v>12</v>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <f>2023-Artist!$E7</f>
+        <v>2022</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A064F3-C50F-4F7F-977E-C8C04FD0B2C9}">
-  <dimension ref="C14:E19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" customWidth="true" width="18.7109375"/>
-    <col min="3" max="3" customWidth="true" width="21.85546875"/>
-    <col min="4" max="4" customWidth="true" width="18.28515625"/>
-    <col min="5" max="5" customWidth="true" width="19.0"/>
-    <col min="6" max="6" customWidth="true" width="12.7109375"/>
-  </cols>
-  <sheetData>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s" s="0">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1887</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="0">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E16" t="s" s="0">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="0">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="D18" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s" s="0">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="D19" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
export data from dataFrame
</commit_message>
<xml_diff>
--- a/WriteTestBook.xlsx
+++ b/WriteTestBook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivannikitka/IdeaProjects/ ObjectStyle/tmp/ApachePOITest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ivan\ObjectStyle\tmpProjects\ApachePOITest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B9C7E8-FE0A-4843-A7AB-FE3945F530E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9EF9E2-852F-4665-A70E-CCCDED09375E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14240" xr2:uid="{D9696ABA-CDAC-264D-8BCE-8FDC23B0FCD9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D9696ABA-CDAC-264D-8BCE-8FDC23B0FCD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Artist" sheetId="1" r:id="rId1"/>
@@ -573,16 +573,16 @@
   <dimension ref="C6:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:F19"/>
+      <selection activeCell="F11" sqref="C8:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
@@ -596,7 +596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" s="7">
         <v>1</v>
       </c>

</xml_diff>